<commit_message>
dynamic and every values are correct
</commit_message>
<xml_diff>
--- a/E-tollAcquiringSettlement/Processing/2025/09/25/ETOLL_ACQUIRING_VOUCHER_250925_N1.xlsx
+++ b/E-tollAcquiringSettlement/Processing/2025/09/25/ETOLL_ACQUIRING_VOUCHER_250925_N1.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1167688440.01</v>
+        <v>233500382.4</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1416977.85</v>
+        <v>54324</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">

</xml_diff>